<commit_message>
Ajout des liens vers le site archives13.fr
- Chaque fonction/categorie a maintenant un lien vers sa page sur archives13.fr
- Le panneau d'info affiche un bouton 'Voir sur archives13.fr' cliquable
- Fonctionne dans les deux vues (Treemap et Arbre)
- URLs ajoutees dans le script de generation des donnees
</commit_message>
<xml_diff>
--- a/data/archives.xlsx
+++ b/data/archives.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,6 +476,11 @@
           <t>Thematique</t>
         </is>
       </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>url</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -510,6 +515,11 @@
           <t>Fonds anciens</t>
         </is>
       </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>https://www.archives13.fr/n/archives-anciennes/n:101</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -544,6 +554,11 @@
           <t>Fonds revolutionnaires</t>
         </is>
       </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>https://www.archives13.fr/n/archives-revolutionnaires/n:102</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -578,6 +593,11 @@
           <t>Fonds publics modernes</t>
         </is>
       </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>https://www.archives13.fr/n/archives-modernes-et-contemporaines/n:103</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -612,6 +632,11 @@
           <t>Sante et assistance</t>
         </is>
       </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>https://www.archives13.fr/n/archives-hospitalieres/n:104</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -646,6 +671,11 @@
           <t>Fonds communaux</t>
         </is>
       </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>https://www.archives13.fr/n/archives-communales-et-intercommunales-deposees/n:105</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -680,6 +710,11 @@
           <t>Fonds prives</t>
         </is>
       </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>https://www.archives13.fr/n/archives-privees/n:106</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -714,6 +749,11 @@
           <t>Images et sons</t>
         </is>
       </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>https://www.archives13.fr/n/fonds-iconographiques-et-audiovisuels/n:107</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -748,6 +788,11 @@
           <t>Documentation</t>
         </is>
       </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>https://www.archives13.fr/n/bibliotheque/n:108</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -782,6 +827,11 @@
           <t>Genealogie</t>
         </is>
       </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>https://www.archives13.fr/n/etat-civil/n:109</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -814,6 +864,11 @@
       <c r="H11" t="inlineStr">
         <is>
           <t>Actes notaries</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>https://www.archives13.fr/n/archives-notariales/n:110</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Ajout du lien vers le moteur de recherche des inventaires
- Nouveau bouton 'Rechercher dans les inventaires' dans le panneau d'info
- Lien vers le moteur de recherche AD13 (980 inventaires, 185 402 notices)
- Style distinct (couleur doree) pour differencier les deux actions
- Fonctionne dans les vues Treemap et Arbre
</commit_message>
<xml_diff>
--- a/data/archives.xlsx
+++ b/data/archives.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,6 +481,11 @@
           <t>url</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>url_recherche</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -520,6 +525,11 @@
           <t>https://www.archives13.fr/n/archives-anciennes/n:101</t>
         </is>
       </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>https://www.archives13.fr/archive/recherche/fonds/n:93</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -559,6 +569,11 @@
           <t>https://www.archives13.fr/n/archives-revolutionnaires/n:102</t>
         </is>
       </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>https://www.archives13.fr/archive/recherche/fonds/n:93</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -598,6 +613,11 @@
           <t>https://www.archives13.fr/n/archives-modernes-et-contemporaines/n:103</t>
         </is>
       </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>https://www.archives13.fr/archive/recherche/fonds/n:93</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -637,6 +657,11 @@
           <t>https://www.archives13.fr/n/archives-hospitalieres/n:104</t>
         </is>
       </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>https://www.archives13.fr/archive/recherche/fonds/n:93</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -676,6 +701,11 @@
           <t>https://www.archives13.fr/n/archives-communales-et-intercommunales-deposees/n:105</t>
         </is>
       </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>https://www.archives13.fr/archive/recherche/fonds/n:93</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -715,6 +745,11 @@
           <t>https://www.archives13.fr/n/archives-privees/n:106</t>
         </is>
       </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>https://www.archives13.fr/archive/recherche/fonds/n:93</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -754,6 +789,11 @@
           <t>https://www.archives13.fr/n/fonds-iconographiques-et-audiovisuels/n:107</t>
         </is>
       </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>https://www.archives13.fr/archive/recherche/fonds/n:93</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -793,6 +833,11 @@
           <t>https://www.archives13.fr/n/bibliotheque/n:108</t>
         </is>
       </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>https://www.archives13.fr/archive/recherche/fonds/n:93</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -832,6 +877,11 @@
           <t>https://www.archives13.fr/n/etat-civil/n:109</t>
         </is>
       </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>https://www.archives13.fr/archive/recherche/fonds/n:93</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -869,6 +919,11 @@
       <c r="I11" t="inlineStr">
         <is>
           <t>https://www.archives13.fr/n/archives-notariales/n:110</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>https://www.archives13.fr/archive/recherche/fonds/n:93</t>
         </is>
       </c>
     </row>

</xml_diff>